<commit_message>
EOH constraint working in monolithic model
</commit_message>
<xml_diff>
--- a/growth_set.xlsx
+++ b/growth_set.xlsx
@@ -791,49 +791,49 @@
         <v>59</v>
       </c>
       <c r="AV2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AW2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AX2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -982,46 +982,46 @@
         <v>59</v>
       </c>
       <c r="AW3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AX3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -1170,46 +1170,46 @@
         <v>59</v>
       </c>
       <c r="AW4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AX4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ4" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1361,43 +1361,43 @@
         <v>59</v>
       </c>
       <c r="AX5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ5" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -1549,43 +1549,43 @@
         <v>59</v>
       </c>
       <c r="AX6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ6" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -1737,43 +1737,43 @@
         <v>58</v>
       </c>
       <c r="AX7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ7" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -1924,46 +1924,46 @@
         <v>59</v>
       </c>
       <c r="AW8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AX8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ8" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -2115,43 +2115,43 @@
         <v>59</v>
       </c>
       <c r="AX9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ9" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
@@ -2303,43 +2303,43 @@
         <v>58</v>
       </c>
       <c r="AX10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AY10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ10" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -2494,40 +2494,40 @@
         <v>59</v>
       </c>
       <c r="AY11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -2682,40 +2682,40 @@
         <v>59</v>
       </c>
       <c r="AY12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AZ12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ12" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -2873,37 +2873,37 @@
         <v>59</v>
       </c>
       <c r="AZ13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BA13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BC13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BF13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BG13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BH13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BJ13" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>